<commit_message>
Latest simplesk plus, windowed context for WSD.
</commit_message>
<xml_diff>
--- a/data/reuters21578/test_results/reuters.xlsx
+++ b/data/reuters21578/test_results/reuters.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
+    <sheet name="zoom" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="13">
   <si>
     <t>alpha</t>
   </si>
@@ -50,6 +51,9 @@
   </si>
   <si>
     <t>WSD: SimpLesk Plus</t>
+  </si>
+  <si>
+    <t>WSD: Simplesk</t>
   </si>
 </sst>
 </file>
@@ -1253,25 +1257,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="52871936"/>
-        <c:axId val="52873472"/>
+        <c:axId val="40748160"/>
+        <c:axId val="40749696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="52871936"/>
+        <c:axId val="40748160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52873472"/>
+        <c:crossAx val="40749696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52873472"/>
+        <c:axId val="40749696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1279,7 +1283,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52871936"/>
+        <c:crossAx val="40748160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1290,7 +1294,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.9327451089890367E-2"/>
+          <c:x val="2.932745108989037E-2"/>
           <c:y val="1.8957341255279508E-2"/>
           <c:w val="0.68602594888404911"/>
           <c:h val="0.10952865133444009"/>
@@ -1301,7 +1305,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -2223,25 +2227,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="52930816"/>
-        <c:axId val="52940800"/>
+        <c:axId val="41204352"/>
+        <c:axId val="41218432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="52930816"/>
+        <c:axId val="41204352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52940800"/>
+        <c:crossAx val="41218432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52940800"/>
+        <c:axId val="41218432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2249,7 +2253,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52930816"/>
+        <c:crossAx val="41204352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2260,10 +2264,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.8859283329602307E-2"/>
-          <c:y val="2.0408163265306121E-2"/>
-          <c:w val="0.67173365999153545"/>
-          <c:h val="0.11164517478793412"/>
+          <c:x val="2.885928332960231E-2"/>
+          <c:y val="2.0408163265306131E-2"/>
+          <c:w val="0.67173365999153578"/>
+          <c:h val="0.11164517478793415"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -2271,7 +2275,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -3193,25 +3197,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="54168576"/>
-        <c:axId val="54182656"/>
+        <c:axId val="41402368"/>
+        <c:axId val="41403904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="54168576"/>
+        <c:axId val="41402368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54182656"/>
+        <c:crossAx val="41403904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54182656"/>
+        <c:axId val="41403904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3219,7 +3223,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54168576"/>
+        <c:crossAx val="41402368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3230,10 +3234,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.3432895260852238E-2"/>
-          <c:y val="1.8779342723004695E-2"/>
-          <c:w val="0.69340257199032918"/>
-          <c:h val="0.10850024028686556"/>
+          <c:x val="2.3432895260852241E-2"/>
+          <c:y val="1.8779342723004692E-2"/>
+          <c:w val="0.69340257199032895"/>
+          <c:h val="0.10850024028686561"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -3241,7 +3245,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -4163,25 +4167,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="54083968"/>
-        <c:axId val="54085504"/>
+        <c:axId val="41309312"/>
+        <c:axId val="41310848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="54083968"/>
+        <c:axId val="41309312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54085504"/>
+        <c:crossAx val="41310848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54085504"/>
+        <c:axId val="41310848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4189,7 +4193,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54083968"/>
+        <c:crossAx val="41309312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4200,10 +4204,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.2316051073325988E-2"/>
-          <c:y val="1.8823529411764704E-2"/>
-          <c:w val="0.67173374161563137"/>
-          <c:h val="0.10799320332788694"/>
+          <c:x val="2.2316051073325991E-2"/>
+          <c:y val="1.8823529411764718E-2"/>
+          <c:w val="0.6717337416156316"/>
+          <c:h val="0.10799320332788698"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -4211,7 +4215,739 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>No WSD</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>zoom!$C$4:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>zoom!$D$4:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.64139371386284305</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.64134718907343302</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.64829972765241295</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.64956087184939804</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.65959582152472296</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.66069433743658201</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.64813983194910096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65911552565004095</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.66514007598394997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.69285005760759499</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.70818272587290898</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.70101819834329604</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.69290075033646903</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.71754639098138095</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.75438285947866301</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.74368091450604601</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.81947866380653001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.71796687740473497</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.73468547676641305</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.72801923258655299</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.70246469610325302</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>WSD</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>zoom!$C$4:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>zoom!$H$4:$H$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.64139371386284305</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.65028807049833404</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.65927281768775603</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.66930906383031696</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.66635852064692602</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.66962833305547098</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.67865414526353296</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.66604322512205505</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.67217051401382499</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.66150790272585602</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.65801743152334402</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.66533997995215199</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.66395804799559999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.66565048990966003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.66978767245668003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.66863091057502799</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.66244765801908301</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.70653944919859102</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.67953275220473397</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.75783633130321204</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.75040662624647403</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="41411328"/>
+        <c:axId val="51098752"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="41411328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="51098752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="51098752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="41411328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.5834116317573961E-2"/>
+          <c:y val="2.0565552699228787E-2"/>
+          <c:w val="0.3068116123673153"/>
+          <c:h val="6.1980851365301702E-2"/>
+        </c:manualLayout>
+      </c:layout>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>No WSD</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>zoom!$C$4:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>zoom!$F$4:$F$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.48964874250613899</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.332476913109154</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.32012669902289997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.31754537183961601</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.44290288876099099</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48080500031205398</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.42858451471922399</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.36462930552455097</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.42152051060272</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.43054869628847098</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.40142679731199699</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.41422407503451297</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.42293298940992702</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.43143111485136398</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.47437089892208401</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.40086116197326299</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.36078621199917899</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.38196341042815801</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.57796629311284498</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.46594221353527299</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.36944664921541598</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>WSD</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>zoom!$C$4:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>zoom!$J$4:$J$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.48964874250613899</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32688001919591098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.45351749226444898</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.28720400940707003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35103096829716901</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26680251653359</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.352982130149186</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.31617668084686001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.47450609542578398</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.34289610340427301</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.37785035038619902</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.346758977705307</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.29034086058696201</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.219801218143264</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.29253613954775198</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.242956299662412</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.29427446258963502</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.30246276654502702</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.40179226957244801</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.44259091277985002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.30687723718347398</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="51127424"/>
+        <c:axId val="51128960"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="51127424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="51128960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="51128960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="51127424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.5834116317573961E-2"/>
+          <c:y val="2.0565552699228787E-2"/>
+          <c:w val="0.30681161236731541"/>
+          <c:h val="6.1980851365301702E-2"/>
+        </c:manualLayout>
+      </c:layout>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -4605,6 +5341,151 @@
 </c:userShapes>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1000125</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.56515</cdr:x>
+      <cdr:y>0</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.76547</cdr:x>
+      <cdr:y>0.10797</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3305175" y="0"/>
+          <a:ext cx="1171575" cy="400051"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1"/>
+            <a:t>Kmeans: F1</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.56515</cdr:x>
+      <cdr:y>0</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.76547</cdr:x>
+      <cdr:y>0.10797</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3305175" y="0"/>
+          <a:ext cx="1171575" cy="400051"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1"/>
+            <a:t>Hierarchical: F1</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4892,8 +5773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AQ25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q55" workbookViewId="0">
-      <selection activeCell="AR8" sqref="AR7:AR8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7830,4 +8711,689 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C1:K25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:11" ht="15.75" thickBot="1"/>
+    <row r="2" spans="3:11" ht="20.25" thickTop="1" thickBot="1">
+      <c r="C2" s="1"/>
+      <c r="D2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="22"/>
+    </row>
+    <row r="3" spans="3:11" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C3" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" ht="15.75" thickTop="1">
+      <c r="C4" s="17">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.64139371386284305</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.92991120548463102</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.48964874250613899</v>
+      </c>
+      <c r="G4" s="10">
+        <v>1.15083916478422</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0.64139371386284305</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.92991120548463102</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.48964874250613899</v>
+      </c>
+      <c r="K4" s="10">
+        <v>1.15083916478422</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11">
+      <c r="C5" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0.64134718907343302</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.92437088015187696</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.332476913109154</v>
+      </c>
+      <c r="G5" s="10">
+        <v>1.34998762010457</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0.65028807049833404</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.90926415426770302</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.32688001919591098</v>
+      </c>
+      <c r="K5" s="10">
+        <v>1.3263320700994601</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11">
+      <c r="C6" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.64829972765241295</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.90462719479970899</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.32012669902289997</v>
+      </c>
+      <c r="G6" s="10">
+        <v>1.4556756497714001</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0.65927281768775603</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.88858106137414306</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.45351749226444898</v>
+      </c>
+      <c r="K6" s="10">
+        <v>1.2011061190008301</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11">
+      <c r="C7" s="17">
+        <v>0.15</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.64956087184939804</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.89854178897148995</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.31754537183961601</v>
+      </c>
+      <c r="G7" s="10">
+        <v>1.2962824986929</v>
+      </c>
+      <c r="H7" s="9">
+        <v>0.66930906383031696</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.87460028102980503</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.28720400940707003</v>
+      </c>
+      <c r="K7" s="10">
+        <v>1.3198259152856</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11">
+      <c r="C8" s="17">
+        <v>0.2</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.65959582152472296</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.88571168342907802</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.44290288876099099</v>
+      </c>
+      <c r="G8" s="10">
+        <v>1.08319619698322</v>
+      </c>
+      <c r="H8" s="9">
+        <v>0.66635852064692602</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.88489152038446095</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.35103096829716901</v>
+      </c>
+      <c r="K8" s="10">
+        <v>1.33258695473585</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11">
+      <c r="C9" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.66069433743658201</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.90029655907024697</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.48080500031205398</v>
+      </c>
+      <c r="G9" s="10">
+        <v>1.0674335444285501</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0.66962833305547098</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.87620475171477996</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.26680251653359</v>
+      </c>
+      <c r="K9" s="10">
+        <v>1.4554048746541499</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11">
+      <c r="C10" s="17">
+        <v>0.3</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0.64813983194910096</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.92832710331008095</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.42858451471922399</v>
+      </c>
+      <c r="G10" s="10">
+        <v>1.19365923261389</v>
+      </c>
+      <c r="H10" s="9">
+        <v>0.67865414526353296</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.86915792904389599</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.352982130149186</v>
+      </c>
+      <c r="K10" s="10">
+        <v>1.0622821780496901</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11">
+      <c r="C11" s="17">
+        <v>0.35</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.65911552565004095</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.91771463488554506</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.36462930552455097</v>
+      </c>
+      <c r="G11" s="10">
+        <v>1.3329258879908901</v>
+      </c>
+      <c r="H11" s="9">
+        <v>0.66604322512205505</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.88288227541439701</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.31617668084686001</v>
+      </c>
+      <c r="K11" s="10">
+        <v>1.17447637270868</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11">
+      <c r="C12" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.66514007598394997</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.90978511613944002</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.42152051060272</v>
+      </c>
+      <c r="G12" s="10">
+        <v>1.3230078522842399</v>
+      </c>
+      <c r="H12" s="9">
+        <v>0.67217051401382499</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.87635184352700002</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.47450609542578398</v>
+      </c>
+      <c r="K12" s="10">
+        <v>1.2227707539025401</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11">
+      <c r="C13" s="17">
+        <v>0.45</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.69285005760759499</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.85249414533626799</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.43054869628847098</v>
+      </c>
+      <c r="G13" s="10">
+        <v>1.24477897932569</v>
+      </c>
+      <c r="H13" s="9">
+        <v>0.66150790272585602</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.89658159436268903</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.34289610340427301</v>
+      </c>
+      <c r="K13" s="10">
+        <v>1.35623210807349</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11">
+      <c r="C14" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0.70818272587290898</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.84049955897296103</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.40142679731199699</v>
+      </c>
+      <c r="G14" s="10">
+        <v>1.0893695592816801</v>
+      </c>
+      <c r="H14" s="9">
+        <v>0.65801743152334402</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.88345815343370804</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.37785035038619902</v>
+      </c>
+      <c r="K14" s="10">
+        <v>1.3168367733300299</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11">
+      <c r="C15" s="17">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.70101819834329604</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.84990057959616905</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.41422407503451297</v>
+      </c>
+      <c r="G15" s="10">
+        <v>1.23051064478278</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0.66533997995215199</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.86220748922346102</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.346758977705307</v>
+      </c>
+      <c r="K15" s="10">
+        <v>1.2918942806386899</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11">
+      <c r="C16" s="17">
+        <v>0.6</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0.69290075033646903</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.850326506001162</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.42293298940992702</v>
+      </c>
+      <c r="G16" s="10">
+        <v>1.1570821685738999</v>
+      </c>
+      <c r="H16" s="9">
+        <v>0.66395804799559999</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.87698069884519603</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.29034086058696201</v>
+      </c>
+      <c r="K16" s="10">
+        <v>1.33628132154058</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11">
+      <c r="C17" s="17">
+        <v>0.65</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0.71754639098138095</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.829227201538698</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.43143111485136398</v>
+      </c>
+      <c r="G17" s="10">
+        <v>1.2615730235487099</v>
+      </c>
+      <c r="H17" s="9">
+        <v>0.66565048990966003</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.86472791895545098</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.219801218143264</v>
+      </c>
+      <c r="K17" s="10">
+        <v>1.47734695833787</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11">
+      <c r="C18" s="17">
+        <v>0.7</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.75438285947866301</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.76405638026804601</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.47437089892208401</v>
+      </c>
+      <c r="G18" s="10">
+        <v>1.0669492865778101</v>
+      </c>
+      <c r="H18" s="9">
+        <v>0.66978767245668003</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.85942851978797297</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.29253613954775198</v>
+      </c>
+      <c r="K18" s="10">
+        <v>1.3762185573279899</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11">
+      <c r="C19" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0.74368091450604601</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.79706937250404497</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.40086116197326299</v>
+      </c>
+      <c r="G19" s="10">
+        <v>1.24523623900811</v>
+      </c>
+      <c r="H19" s="9">
+        <v>0.66863091057502799</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.86220909064832396</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0.242956299662412</v>
+      </c>
+      <c r="K19" s="10">
+        <v>1.3793337662804299</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11">
+      <c r="C20" s="17">
+        <v>0.8</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0.81947866380653001</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.59484427348606295</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.36078621199917899</v>
+      </c>
+      <c r="G20" s="10">
+        <v>1.2434292413881001</v>
+      </c>
+      <c r="H20" s="9">
+        <v>0.66244765801908301</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0.866146158045627</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.29427446258963502</v>
+      </c>
+      <c r="K20" s="10">
+        <v>1.3528562744057899</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11">
+      <c r="C21" s="17">
+        <v>0.85</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.71796687740473497</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.85225107443251402</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.38196341042815801</v>
+      </c>
+      <c r="G21" s="10">
+        <v>1.23284188164078</v>
+      </c>
+      <c r="H21" s="9">
+        <v>0.70653944919859102</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.84305269050007603</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0.30246276654502702</v>
+      </c>
+      <c r="K21" s="10">
+        <v>1.2915483113549799</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11">
+      <c r="C22" s="17">
+        <v>0.9</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0.73468547676641305</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.822373207498724</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.57796629311284498</v>
+      </c>
+      <c r="G22" s="10">
+        <v>1.1139539818784301</v>
+      </c>
+      <c r="H22" s="9">
+        <v>0.67953275220473397</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.872780602537511</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0.40179226957244801</v>
+      </c>
+      <c r="K22" s="10">
+        <v>1.2317369596834999</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11">
+      <c r="C23" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0.72801923258655299</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.84361692794484999</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.46594221353527299</v>
+      </c>
+      <c r="G23" s="10">
+        <v>1.1765004310396501</v>
+      </c>
+      <c r="H23" s="9">
+        <v>0.75783633130321204</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0.70327418975062495</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.44259091277985002</v>
+      </c>
+      <c r="K23" s="10">
+        <v>1.1723701720016599</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" ht="15.75" thickBot="1">
+      <c r="C24" s="18">
+        <v>1</v>
+      </c>
+      <c r="D24" s="11">
+        <v>0.70246469610325302</v>
+      </c>
+      <c r="E24" s="12">
+        <v>0.89801032864762098</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0.36944664921541598</v>
+      </c>
+      <c r="G24" s="13">
+        <v>1.3659813478724401</v>
+      </c>
+      <c r="H24" s="11">
+        <v>0.75040662624647403</v>
+      </c>
+      <c r="I24" s="12">
+        <v>0.72550702828692304</v>
+      </c>
+      <c r="J24" s="12">
+        <v>0.30687723718347398</v>
+      </c>
+      <c r="K24" s="13">
+        <v>1.49911991060544</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" ht="15.75" thickTop="1"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:K2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>